<commit_message>
Started v4.2 with charge component changes and discharge LED
</commit_message>
<xml_diff>
--- a/BMS/Project Outputs for Battman/Battman.xlsx
+++ b/BMS/Project Outputs for Battman/Battman.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="317">
   <si>
     <t>Designator</t>
   </si>
@@ -230,6 +230,15 @@
     <t>10nF 50V 10% 0402 (1005 Metric)</t>
   </si>
   <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>GRM1555C1H102JA01D</t>
+  </si>
+  <si>
+    <t>1nF 50V 5% 0402 (1005 Metric)</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -266,13 +275,13 @@
     <t>NXP</t>
   </si>
   <si>
-    <t>PTVS24VS1UTR,115</t>
+    <t>PTVS40VS1UTR,115</t>
   </si>
   <si>
     <t>SOD-123W</t>
   </si>
   <si>
-    <t>D4, D7, D13</t>
+    <t>D4, D7, D13, D19</t>
   </si>
   <si>
     <t>Lite-On Inc.</t>
@@ -284,13 +293,16 @@
     <t>D5</t>
   </si>
   <si>
-    <t>Comchip Technology</t>
-  </si>
-  <si>
-    <t>CDBB560-HF</t>
-  </si>
-  <si>
-    <t>DO-214AA</t>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>FSV10120V</t>
+  </si>
+  <si>
+    <t>TO-277-3</t>
+  </si>
+  <si>
+    <t>Schottky Diodes &amp; Rectifiers 10 Amp 120V Schottky Rectifier</t>
   </si>
   <si>
     <t>D6, D16, D17</t>
@@ -485,10 +497,10 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>SI4190ADY-T1-GE3</t>
-  </si>
-  <si>
-    <t>SO-8</t>
+    <t>SIR664DP-T1-GE3</t>
+  </si>
+  <si>
+    <t>PowerPAK-8</t>
   </si>
   <si>
     <t>Q3_1, Q3_2, Q3_3, Q3_4, Q3_5, Q3_6, Q3_7, Q3_8, Q3_9, Q3_10, Q3_11, Q3_12, Q5, Q9</t>
@@ -524,7 +536,10 @@
     <t>Q6</t>
   </si>
   <si>
-    <t>PMV16XNR</t>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>SSM3K341R,LF</t>
   </si>
   <si>
     <t>SOT-23-3</t>
@@ -599,7 +614,7 @@
     <t>1K5 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>R14, R17, R18, R28, R52</t>
+    <t>R14, R17, R18, R28, R40, R52</t>
   </si>
   <si>
     <t>RK73H1ETTP4701F</t>
@@ -608,7 +623,7 @@
     <t>4K7 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>Bottom, Bottom, Bottom, Top, Bottom</t>
+    <t>Bottom, Bottom, Bottom, Top, Bottom, Bottom</t>
   </si>
   <si>
     <t>R15, R16</t>
@@ -620,7 +635,7 @@
     <t>2K2 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>R19, R23, R24, R40, R41, R43, R45, R47, R48, R58</t>
+    <t>R19, R23, R24, R41, R43, R45, R47, R48, R58</t>
   </si>
   <si>
     <t>RK73H1ETTP1002F</t>
@@ -629,7 +644,7 @@
     <t>10K 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>Top, Bottom, Top, Bottom, Bottom, Bottom, Bottom, Bottom, Bottom, Bottom</t>
+    <t>Top, Bottom, Top, Bottom, Bottom, Bottom, Bottom, Bottom, Bottom</t>
   </si>
   <si>
     <t>R20, R21</t>
@@ -737,10 +752,10 @@
     <t>R38</t>
   </si>
   <si>
-    <t>RK73H1ETTP4702F</t>
-  </si>
-  <si>
-    <t>47K 0.063W 1% 0402 (1005 Metric)</t>
+    <t>RK73H1ETTP3902F</t>
+  </si>
+  <si>
+    <t>39K 0.063W 1% 0402 (1005 Metric)</t>
   </si>
   <si>
     <t>R39, R46, R49</t>
@@ -801,6 +816,15 @@
   </si>
   <si>
     <t>10K 0.25W 5% 0603 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>RCS060310K0FKEA</t>
+  </si>
+  <si>
+    <t>10K 0.25W 1% 0603 (1005 Metric)</t>
   </si>
   <si>
     <t>U1</t>
@@ -1436,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1851,16 +1875,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>12</v>
@@ -1868,45 +1892,45 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="F19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G19" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>28</v>
@@ -1914,25 +1938,25 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="3">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1940,7 +1964,7 @@
         <v>85</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>86</v>
@@ -1949,10 +1973,10 @@
         <v>87</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>12</v>
@@ -1960,25 +1984,25 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="3">
-        <v>3</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G23" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1986,7 +2010,7 @@
         <v>93</v>
       </c>
       <c r="B24" s="3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>94</v>
@@ -1998,30 +2022,30 @@
         <v>96</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="3">
+        <v>12</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="3">
-        <v>12</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>12</v>
@@ -2029,22 +2053,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B26" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>12</v>
@@ -2052,25 +2076,25 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B27" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2078,19 +2102,19 @@
         <v>107</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>28</v>
@@ -2098,22 +2122,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B29" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>28</v>
@@ -2124,7 +2148,7 @@
         <v>113</v>
       </c>
       <c r="B30" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>114</v>
@@ -2133,13 +2157,13 @@
         <v>115</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G30" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2147,19 +2171,19 @@
         <v>117</v>
       </c>
       <c r="B31" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>12</v>
@@ -2167,22 +2191,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B32" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>12</v>
@@ -2190,22 +2214,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="F33" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>12</v>
@@ -2219,16 +2243,16 @@
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>12</v>
@@ -2236,22 +2260,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>131</v>
       </c>
       <c r="E35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>12</v>
@@ -2259,13 +2283,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>135</v>
@@ -2288,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>139</v>
@@ -2300,7 +2324,7 @@
         <v>141</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2311,16 +2335,16 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>28</v>
@@ -2328,22 +2352,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="3">
-        <v>6</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>28</v>
@@ -2351,13 +2375,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" s="3">
+        <v>6</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>153</v>
@@ -2366,21 +2390,21 @@
         <v>154</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B41" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>157</v>
@@ -2389,33 +2413,33 @@
         <v>158</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" s="3">
+        <v>14</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="E42" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="F42" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="G42" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2426,39 +2450,39 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>12</v>
@@ -2466,22 +2490,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B45" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>172</v>
+        <v>94</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>12</v>
@@ -2489,91 +2513,91 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B46" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B47" s="3">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B48" s="3">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B49" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>28</v>
@@ -2581,22 +2605,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>28</v>
@@ -2604,114 +2628,114 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B51" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>194</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>28</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B53" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>201</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B54" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B55" s="3">
         <v>2</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>28</v>
@@ -2719,68 +2743,68 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B56" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B58" s="3">
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>28</v>
@@ -2788,114 +2812,114 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B59" s="3">
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B60" s="3">
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B61" s="3">
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B62" s="3">
         <v>1</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B63" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>28</v>
@@ -2903,22 +2927,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B64" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>28</v>
@@ -2926,22 +2950,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B65" s="3">
         <v>1</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>28</v>
@@ -2949,22 +2973,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B66" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>28</v>
@@ -2972,71 +2996,71 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B67" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B68" s="3">
         <v>1</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B69" s="3">
         <v>1</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>249</v>
+        <v>177</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>252</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -3044,19 +3068,19 @@
         <v>253</v>
       </c>
       <c r="B70" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G70" s="8" t="s">
         <v>12</v>
@@ -3064,68 +3088,68 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B71" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>90</v>
+        <v>177</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B72" s="3">
         <v>1</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>260</v>
+        <v>94</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>262</v>
+        <v>63</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>77</v>
+        <v>263</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B73" s="3">
         <v>1</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>264</v>
+        <v>94</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>265</v>
       </c>
       <c r="E73" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>28</v>
@@ -3148,7 +3172,7 @@
         <v>270</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>271</v>
+        <v>80</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>12</v>
@@ -3156,22 +3180,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B75" s="3">
-        <v>1</v>
-      </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="E75" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E75" s="6" t="s">
-        <v>270</v>
-      </c>
       <c r="F75" s="7" t="s">
-        <v>275</v>
+        <v>80</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>28</v>
@@ -3179,13 +3203,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="B76" s="3">
-        <v>1</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>273</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>277</v>
@@ -3208,13 +3232,13 @@
         <v>1</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>283</v>
@@ -3231,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>285</v>
@@ -3243,7 +3267,7 @@
         <v>287</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -3254,7 +3278,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>289</v>
@@ -3277,19 +3301,19 @@
         <v>1</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="E80" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="F80" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="F80" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G80" s="8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -3300,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>297</v>
@@ -3332,10 +3356,10 @@
         <v>303</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -3346,18 +3370,64 @@
         <v>1</v>
       </c>
       <c r="C83" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="F83" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G85" s="8" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>